<commit_message>
Codigo a pegar en el MAIN
Se llama Codigo_Control_DC_Completo solamente es pegar las funciones y
ya
</commit_message>
<xml_diff>
--- a/Bioimpedanciometro_Sketch_Funcional_3.0/Datos Bioimpedanciometro.xlsx
+++ b/Bioimpedanciometro_Sketch_Funcional_3.0/Datos Bioimpedanciometro.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
   <si>
     <t>Valor medido</t>
   </si>
@@ -171,12 +171,21 @@
   <si>
     <t>19382.31</t>
   </si>
+  <si>
+    <t>Valor de Farbica</t>
+  </si>
+  <si>
+    <t>Valor Sensado</t>
+  </si>
+  <si>
+    <t>Error Porcentual</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +213,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -339,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,23 +395,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,6 +420,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,6 +474,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,11 +649,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-754795328"/>
-        <c:axId val="-754795872"/>
+        <c:axId val="-841703744"/>
+        <c:axId val="-841700480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-754795328"/>
+        <c:axId val="-841703744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -740,12 +767,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-754795872"/>
+        <c:crossAx val="-841700480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-754795872"/>
+        <c:axId val="-841700480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +900,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-754795328"/>
+        <c:crossAx val="-841703744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1182,11 +1209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-751682976"/>
-        <c:axId val="-751676448"/>
+        <c:axId val="-775557504"/>
+        <c:axId val="-775556416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-751682976"/>
+        <c:axId val="-775557504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1243,12 +1270,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-751676448"/>
+        <c:crossAx val="-775556416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-751676448"/>
+        <c:axId val="-775556416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,7 +1332,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-751682976"/>
+        <c:crossAx val="-775557504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1534,11 +1561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759360112"/>
-        <c:axId val="-759368272"/>
+        <c:axId val="-774928032"/>
+        <c:axId val="-774931840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759360112"/>
+        <c:axId val="-774928032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,12 +1622,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759368272"/>
+        <c:crossAx val="-774931840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759368272"/>
+        <c:axId val="-774931840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1684,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759360112"/>
+        <c:crossAx val="-774928032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1886,11 +1913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759369360"/>
-        <c:axId val="-759366640"/>
+        <c:axId val="-774930208"/>
+        <c:axId val="-774927488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759369360"/>
+        <c:axId val="-774930208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1947,12 +1974,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759366640"/>
+        <c:crossAx val="-774927488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759366640"/>
+        <c:axId val="-774927488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2009,7 +2036,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759369360"/>
+        <c:crossAx val="-774930208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2238,11 +2265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759373712"/>
-        <c:axId val="-759371536"/>
+        <c:axId val="-774929664"/>
+        <c:axId val="-774929120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759373712"/>
+        <c:axId val="-774929664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,12 +2326,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759371536"/>
+        <c:crossAx val="-774929120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759371536"/>
+        <c:axId val="-774929120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2361,7 +2388,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759373712"/>
+        <c:crossAx val="-774929664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2473,26 +2500,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2656,11 +2663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-746777296"/>
-        <c:axId val="-746790896"/>
+        <c:axId val="-773917680"/>
+        <c:axId val="-773919312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-746777296"/>
+        <c:axId val="-773917680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2715,26 +2722,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2773,12 +2760,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-746790896"/>
+        <c:crossAx val="-773919312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-746790896"/>
+        <c:axId val="-773919312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,26 +2820,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2891,7 +2858,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-746777296"/>
+        <c:crossAx val="-773917680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3147,11 +3114,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759364464"/>
-        <c:axId val="-759360656"/>
+        <c:axId val="-773910064"/>
+        <c:axId val="-773923664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759364464"/>
+        <c:axId val="-773910064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3203,12 +3170,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759360656"/>
+        <c:crossAx val="-773923664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759360656"/>
+        <c:axId val="-773923664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3264,7 +3231,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759364464"/>
+        <c:crossAx val="-773910064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3509,11 +3476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837144112"/>
-        <c:axId val="-837143568"/>
+        <c:axId val="-773922576"/>
+        <c:axId val="-773909520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837144112"/>
+        <c:axId val="-773922576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3565,12 +3532,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837143568"/>
+        <c:crossAx val="-773909520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837143568"/>
+        <c:axId val="-773909520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3626,7 +3593,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837144112"/>
+        <c:crossAx val="-773922576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3871,11 +3838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837141936"/>
-        <c:axId val="-837144656"/>
+        <c:axId val="-773920944"/>
+        <c:axId val="-773920400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837141936"/>
+        <c:axId val="-773920944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3927,12 +3894,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837144656"/>
+        <c:crossAx val="-773920400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837144656"/>
+        <c:axId val="-773920400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3988,7 +3955,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837141936"/>
+        <c:crossAx val="-773920944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4233,11 +4200,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-837147920"/>
-        <c:axId val="-837147376"/>
+        <c:axId val="-773916048"/>
+        <c:axId val="-773917136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-837147920"/>
+        <c:axId val="-773916048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4289,12 +4256,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837147376"/>
+        <c:crossAx val="-773917136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-837147376"/>
+        <c:axId val="-773917136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4350,7 +4317,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-837147920"/>
+        <c:crossAx val="-773916048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4612,11 +4579,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-834351856"/>
-        <c:axId val="-834344240"/>
+        <c:axId val="-841698848"/>
+        <c:axId val="-841698304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-834351856"/>
+        <c:axId val="-841698848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4659,7 +4626,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834344240"/>
+        <c:crossAx val="-841698304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4667,7 +4634,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-834344240"/>
+        <c:axId val="-841698304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4718,7 +4685,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834351856"/>
+        <c:crossAx val="-841698848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4994,11 +4961,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-834339888"/>
-        <c:axId val="-834337168"/>
+        <c:axId val="-875209696"/>
+        <c:axId val="-775561856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-834339888"/>
+        <c:axId val="-875209696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5041,7 +5008,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834337168"/>
+        <c:crossAx val="-775561856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5049,7 +5016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-834337168"/>
+        <c:axId val="-775561856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5100,7 +5067,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834339888"/>
+        <c:crossAx val="-875209696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5384,11 +5351,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-834350768"/>
-        <c:axId val="-834350224"/>
+        <c:axId val="-775552608"/>
+        <c:axId val="-775561312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-834350768"/>
+        <c:axId val="-775552608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5440,12 +5407,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834350224"/>
+        <c:crossAx val="-775561312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-834350224"/>
+        <c:axId val="-775561312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5501,7 +5468,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834350768"/>
+        <c:crossAx val="-775552608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5742,11 +5709,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-834349136"/>
-        <c:axId val="-834347504"/>
+        <c:axId val="-775554240"/>
+        <c:axId val="-775552064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-834349136"/>
+        <c:axId val="-775554240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5798,12 +5765,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834347504"/>
+        <c:crossAx val="-775552064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-834347504"/>
+        <c:axId val="-775552064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5859,7 +5826,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834349136"/>
+        <c:crossAx val="-775554240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6121,11 +6088,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-834346416"/>
-        <c:axId val="-834345872"/>
+        <c:axId val="-775553152"/>
+        <c:axId val="-775550976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-834346416"/>
+        <c:axId val="-775553152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6177,12 +6144,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834345872"/>
+        <c:crossAx val="-775550976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-834345872"/>
+        <c:axId val="-775550976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6238,7 +6205,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-834346416"/>
+        <c:crossAx val="-775553152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6479,11 +6446,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1052436640"/>
-        <c:axId val="-759370992"/>
+        <c:axId val="-775550432"/>
+        <c:axId val="-775565664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1052436640"/>
+        <c:axId val="-775550432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6535,12 +6502,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759370992"/>
+        <c:crossAx val="-775565664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759370992"/>
+        <c:axId val="-775565664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6596,7 +6563,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1052436640"/>
+        <c:crossAx val="-775550432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6837,11 +6804,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759362832"/>
-        <c:axId val="-759362288"/>
+        <c:axId val="-775559680"/>
+        <c:axId val="-775558048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759362832"/>
+        <c:axId val="-775559680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6893,12 +6860,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759362288"/>
+        <c:crossAx val="-775558048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759362288"/>
+        <c:axId val="-775558048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6954,7 +6921,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759362832"/>
+        <c:crossAx val="-775559680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7195,11 +7162,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759359568"/>
-        <c:axId val="-759366096"/>
+        <c:axId val="-775559136"/>
+        <c:axId val="-775562944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759359568"/>
+        <c:axId val="-775559136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7251,12 +7218,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759366096"/>
+        <c:crossAx val="-775562944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759366096"/>
+        <c:axId val="-775562944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7312,7 +7279,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759359568"/>
+        <c:crossAx val="-775559136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7724,46 +7691,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -10805,557 +10732,6 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11893,7 +11269,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12431,7 +11807,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12969,7 +12345,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18155,16 +17531,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18576,8 +17952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18594,460 +17970,460 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="15">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="24">
         <v>140</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="25">
         <v>135</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="25">
         <v>483</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="25">
         <v>615</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="25">
         <v>139</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="25">
         <v>72</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="25">
         <v>6318</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="25">
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="15">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="24">
         <v>163</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="25">
         <v>131</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="25">
         <v>472</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="25">
         <v>651</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="25">
         <v>131</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="25">
         <v>67</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="25">
         <v>6317</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="25">
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="15">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="24">
         <v>149</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="25">
         <v>129</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="25">
         <v>507</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="25">
         <v>626</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="25">
         <v>202</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="25">
         <v>42</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="25">
         <v>6329</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="25">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="15">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="24">
         <v>135</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="25">
         <v>134</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="25">
         <v>510</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="25">
         <v>614</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="25">
         <v>177</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="25">
         <v>45</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="25">
         <v>6321</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="25">
         <v>390</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="15">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="24">
         <v>149</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="25">
         <v>134</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="25">
         <v>459</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="25">
         <v>683</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="25">
         <v>140</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="25">
         <v>60</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="25">
         <v>6316</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="25">
         <v>462</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="15">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="24">
         <v>140</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="25">
         <v>151</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="25">
         <v>492</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="25">
         <v>642</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="25">
         <v>145</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="25">
         <v>65</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="25">
         <v>6335</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="25">
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="15">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="24">
         <v>134</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="25">
         <v>154</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="25">
         <v>507</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="25">
         <v>655</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="25">
         <v>188</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="25">
         <v>61</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="25">
         <v>6338</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="25">
         <v>388</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="15">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="24">
         <v>183</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="25">
         <v>164</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="25">
         <v>439</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="25">
         <v>654</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="25">
         <v>179</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="25">
         <v>48</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="25">
         <v>6330</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="25">
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="15">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="24">
         <v>171</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="25">
         <v>141</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="25">
         <v>427</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="25">
         <v>649</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="25">
         <v>176</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="25">
         <v>57</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="25">
         <v>6327</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="25">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="15">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="24">
         <v>180</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="25">
         <v>170</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="25">
         <v>476</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="25">
         <v>610</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="25">
         <v>151</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="25">
         <v>66</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="25">
         <v>6326</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="25">
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="15">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="24">
         <v>139</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="25">
         <v>134</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="25">
         <v>486</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="25">
         <v>661</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="25">
         <v>165</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="25">
         <v>79</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="25">
         <v>6320</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="25">
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="13" t="s">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="16">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="29">
         <f t="shared" ref="B16:I16" si="0">(B4+B5+B6+B7+B8+B9+B10+B11+B12+B13)/10</f>
         <v>154.4</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="30">
         <f t="shared" si="0"/>
         <v>144.30000000000001</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="30">
         <f t="shared" si="0"/>
         <v>477.2</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="30">
         <f t="shared" si="0"/>
         <v>639.9</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="30">
         <f t="shared" si="0"/>
         <v>162.80000000000001</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="30">
         <f t="shared" si="0"/>
         <v>58.3</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="30">
         <f t="shared" si="0"/>
         <v>6325.7</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="30">
         <f t="shared" si="0"/>
         <v>306.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="30">
         <f>MAX(B4:B14)</f>
         <v>183</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="30">
         <f t="shared" ref="C17:I17" si="1">MAX(C4:C14)</f>
         <v>170</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="30">
         <f t="shared" si="1"/>
         <v>510</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="30">
         <f t="shared" si="1"/>
         <v>683</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="31">
         <f t="shared" si="1"/>
         <v>202</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="30">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="30">
         <f t="shared" si="1"/>
         <v>6338</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="30">
         <f t="shared" si="1"/>
         <v>462</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="30">
         <f>MIN(B4:B14)</f>
         <v>134</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="30">
         <f t="shared" ref="C18:I18" si="2">MIN(C4:C14)</f>
         <v>129</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="32">
         <f t="shared" si="2"/>
         <v>427</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="30">
         <f t="shared" si="2"/>
         <v>610</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="30">
         <f t="shared" si="2"/>
         <v>131</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="30">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="30">
         <f t="shared" si="2"/>
         <v>6316</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="30">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
@@ -19142,22 +18518,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="H3" s="37" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="H3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -19724,12 +19100,12 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
@@ -19869,12 +19245,12 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="5" t="s">
         <v>7</v>
       </c>
@@ -20015,12 +19391,12 @@
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="5" t="s">
         <v>7</v>
       </c>
@@ -20170,12 +19546,12 @@
       <c r="B30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
       <c r="G30" s="5" t="s">
         <v>7</v>
       </c>
@@ -20291,38 +19667,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:Q32"/>
+  <dimension ref="B5:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="12" t="s">
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>240</v>
       </c>
@@ -20351,7 +19730,7 @@
         <v>-1.3172291666667966</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>180</v>
       </c>
@@ -20380,7 +19759,7 @@
         <v>5.8522083333334907</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>120</v>
       </c>
@@ -20409,49 +19788,68 @@
         <v>-4.741124999999708</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J9">
         <v>14181</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P11" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J12">
         <v>14229</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="25">
         <v>120</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="25">
         <v>125.68</v>
       </c>
+      <c r="R12" s="30">
+        <f>((Q12-P12)/P12)*100</f>
+        <v>4.7333333333333387</v>
+      </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="12" t="s">
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="25">
         <v>180</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="25">
         <v>169.46</v>
       </c>
+      <c r="R13" s="30">
+        <f t="shared" ref="R13:R23" si="3">((Q13-P13)/P13)*100</f>
+        <v>-5.8555555555555516</v>
+      </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>530</v>
       </c>
@@ -20479,14 +19877,18 @@
         <f>((B14-H14)/B14)*100</f>
         <v>-1.7789150943394387</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="25">
         <v>240</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14" s="25">
         <v>243.16</v>
       </c>
+      <c r="R14" s="30">
+        <f t="shared" si="3"/>
+        <v>1.3166666666666653</v>
+      </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>470</v>
       </c>
@@ -20503,25 +19905,29 @@
         <v>14068</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" ref="G15:G16" si="3">(C15+D15+E15+F15)/4</f>
+        <f t="shared" ref="G15:G16" si="4">(C15+D15+E15+F15)/4</f>
         <v>14084.25</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ref="H15:H16" si="4">(-1.143*G15)+16544</f>
+        <f t="shared" ref="H15:H16" si="5">(-1.143*G15)+16544</f>
         <v>445.70225000000028</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" ref="I15:I16" si="5">((B15-H15)/B15)*100</f>
+        <f t="shared" ref="I15:I16" si="6">((B15-H15)/B15)*100</f>
         <v>5.1697340425531326</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="25">
         <v>360</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="25">
         <v>372.26</v>
       </c>
+      <c r="R15" s="30">
+        <f t="shared" si="3"/>
+        <v>3.4055555555555532</v>
+      </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>360</v>
       </c>
@@ -20538,99 +19944,123 @@
         <v>14205</v>
       </c>
       <c r="G16" s="3">
+        <f t="shared" si="4"/>
+        <v>14148.5</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="5"/>
+        <v>372.26449999999932</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="6"/>
+        <v>-3.406805555555366</v>
+      </c>
+      <c r="P16" s="25">
+        <v>470</v>
+      </c>
+      <c r="Q16" s="25">
+        <v>445.7</v>
+      </c>
+      <c r="R16" s="30">
         <f t="shared" si="3"/>
-        <v>14148.5</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="4"/>
-        <v>372.26449999999932</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="5"/>
-        <v>-3.406805555555366</v>
-      </c>
-      <c r="P16" s="3">
-        <v>470</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>445.7</v>
+        <v>-5.1702127659574497</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J17">
         <v>13984</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="25">
         <v>530</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="Q17" s="25">
         <v>539.41999999999996</v>
       </c>
+      <c r="R17" s="30">
+        <f t="shared" si="3"/>
+        <v>1.7773584905660298</v>
+      </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="P18" s="3">
+    <row r="18" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P18" s="25">
         <v>590</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18" s="25">
         <v>589.5</v>
       </c>
+      <c r="R18" s="30">
+        <f t="shared" si="3"/>
+        <v>-8.4745762711864403E-2</v>
+      </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="P19" s="3">
+    <row r="19" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P19" s="25">
         <v>650</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q19" s="25">
         <v>650.78</v>
       </c>
+      <c r="R19" s="30">
+        <f t="shared" si="3"/>
+        <v>0.1199999999999958</v>
+      </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J20">
         <v>13963</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="25">
         <v>710</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q20" s="25">
         <v>709.49</v>
       </c>
+      <c r="R20" s="30">
+        <f t="shared" si="3"/>
+        <v>-7.1830985915491682E-2</v>
+      </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+    <row r="21" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="12" t="s">
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="25">
         <v>830</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="Q21" s="25">
         <v>841.21</v>
       </c>
+      <c r="R21" s="30">
+        <f t="shared" si="3"/>
+        <v>1.3506024096385585</v>
+      </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>710</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="16">
         <v>13795</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="16">
         <v>13791</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="16">
         <v>13696</v>
       </c>
       <c r="F22" s="9">
@@ -20648,14 +20078,18 @@
         <f>((B22-H22)/B22)*100</f>
         <v>7.171478873228615E-2</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22" s="25">
         <v>940</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="Q22" s="25">
         <v>918.97</v>
       </c>
+      <c r="R22" s="30">
+        <f t="shared" si="3"/>
+        <v>-2.2372340425531885</v>
+      </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>650</v>
       </c>
@@ -20672,25 +20106,29 @@
         <v>13827</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" ref="G23:G24" si="6">(C23+D23+E23+F23)/4</f>
+        <f t="shared" ref="G23:G24" si="7">(C23+D23+E23+F23)/4</f>
         <v>13848.75</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" ref="H23:H24" si="7">(-0.7933*G23)+11637</f>
+        <f t="shared" ref="H23:H24" si="8">(-0.7933*G23)+11637</f>
         <v>650.78662500000064</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" ref="I23:I24" si="8">((B23-H23)/B23)*100</f>
+        <f t="shared" ref="I23:I24" si="9">((B23-H23)/B23)*100</f>
         <v>-0.12101923076932929</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23" s="25">
         <v>1000</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="Q23" s="25">
         <v>1009.61</v>
       </c>
+      <c r="R23" s="30">
+        <f t="shared" si="3"/>
+        <v>0.96100000000000141</v>
+      </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>590</v>
       </c>
@@ -20707,54 +20145,54 @@
         <v>13890</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13926</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>589.5041999999994</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8.4033898305186358E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J25">
         <v>13711</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J28">
         <v>13816</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="12" t="s">
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>1000</v>
       </c>
@@ -20783,7 +20221,7 @@
         <v>-0.96178499999996347</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>940</v>
       </c>
@@ -20800,19 +20238,19 @@
         <v>13442</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" ref="G31:G32" si="9">(C31+D31+E31+F31)/4</f>
+        <f t="shared" ref="G31:G32" si="10">(C31+D31+E31+F31)/4</f>
         <v>13492.5</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" ref="H31:H32" si="10">(-0.4906*G31)+7538.4</f>
+        <f t="shared" ref="H31:H32" si="11">(-0.4906*G31)+7538.4</f>
         <v>918.97949999999946</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" ref="I31:I32" si="11">((B31-H31)/B31)*100</f>
+        <f t="shared" ref="I31:I32" si="12">((B31-H31)/B31)*100</f>
         <v>2.2362234042553766</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>830</v>
       </c>
@@ -20829,15 +20267,15 @@
         <v>13596</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13651</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>841.21939999999995</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-1.3517349397590301</v>
       </c>
     </row>
@@ -20849,7 +20287,8 @@
     <mergeCell ref="C29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20857,7 +20296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:U57"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
@@ -20867,60 +20306,60 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="13">
         <v>100</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="14">
         <v>150</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="15">
         <v>200</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="15">
         <v>250</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="18">
         <v>300</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="12">
         <v>350</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="12">
         <v>400</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="17">
         <v>500</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="17">
         <v>550</v>
       </c>
-      <c r="N5" s="26">
+      <c r="N5" s="17">
         <v>600</v>
       </c>
-      <c r="O5" s="26">
+      <c r="O5" s="17">
         <v>700</v>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="17">
         <v>750</v>
       </c>
-      <c r="R5" s="26">
+      <c r="R5" s="17">
         <v>800</v>
       </c>
-      <c r="S5" s="26">
+      <c r="S5" s="17">
         <v>900</v>
       </c>
-      <c r="T5" s="26">
+      <c r="T5" s="17">
         <v>1000</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="17">
         <v>1100</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3">
@@ -20956,7 +20395,7 @@
       <c r="O6" s="3">
         <v>19473</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="19">
         <v>19473</v>
       </c>
       <c r="R6" s="3">
@@ -20973,7 +20412,7 @@
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="3">
         <v>20164</v>
       </c>
@@ -21007,7 +20446,7 @@
       <c r="O7" s="3">
         <v>19472</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="19">
         <v>19475</v>
       </c>
       <c r="R7" s="3">
@@ -21024,7 +20463,7 @@
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="38"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="3">
         <v>20128</v>
       </c>
@@ -21058,7 +20497,7 @@
       <c r="O8" s="3">
         <v>19514</v>
       </c>
-      <c r="P8" s="28">
+      <c r="P8" s="19">
         <v>19473</v>
       </c>
       <c r="R8" s="3">
@@ -21075,7 +20514,7 @@
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="3">
         <v>20138</v>
       </c>
@@ -21109,7 +20548,7 @@
       <c r="O9" s="3">
         <v>19481</v>
       </c>
-      <c r="P9" s="28">
+      <c r="P9" s="19">
         <v>19462</v>
       </c>
       <c r="R9" s="3">
@@ -21126,7 +20565,7 @@
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="3">
         <v>20196</v>
       </c>
@@ -21160,7 +20599,7 @@
       <c r="O10" s="3">
         <v>19497</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="19">
         <v>19466</v>
       </c>
       <c r="R10" s="3">
@@ -21177,7 +20616,7 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="3">
         <v>20120</v>
       </c>
@@ -21211,7 +20650,7 @@
       <c r="O11" s="3">
         <v>19480</v>
       </c>
-      <c r="P11" s="28">
+      <c r="P11" s="19">
         <v>19489</v>
       </c>
       <c r="R11" s="3">
@@ -21228,7 +20667,7 @@
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="3">
         <v>20132</v>
       </c>
@@ -21262,7 +20701,7 @@
       <c r="O12" s="3">
         <v>19478</v>
       </c>
-      <c r="P12" s="28">
+      <c r="P12" s="19">
         <v>19457</v>
       </c>
       <c r="R12" s="3">
@@ -21279,7 +20718,7 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="3">
         <v>20183</v>
       </c>
@@ -21313,7 +20752,7 @@
       <c r="O13" s="3">
         <v>19487</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="19">
         <v>19470</v>
       </c>
       <c r="R13" s="3">
@@ -21330,7 +20769,7 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="3">
         <v>20129</v>
       </c>
@@ -21364,7 +20803,7 @@
       <c r="O14" s="3">
         <v>19476</v>
       </c>
-      <c r="P14" s="28">
+      <c r="P14" s="19">
         <v>19456</v>
       </c>
       <c r="R14" s="3">
@@ -21381,7 +20820,7 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="3">
         <v>20131</v>
       </c>
@@ -21415,7 +20854,7 @@
       <c r="O15" s="3">
         <v>19480</v>
       </c>
-      <c r="P15" s="28">
+      <c r="P15" s="19">
         <v>19484</v>
       </c>
       <c r="R15" s="3">
@@ -21432,7 +20871,7 @@
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="3">
         <v>20133</v>
       </c>
@@ -21466,7 +20905,7 @@
       <c r="O16" s="3">
         <v>19508</v>
       </c>
-      <c r="P16" s="28">
+      <c r="P16" s="19">
         <v>19463</v>
       </c>
       <c r="R16" s="3">
@@ -21483,7 +20922,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="3">
         <v>20181</v>
       </c>
@@ -21517,7 +20956,7 @@
       <c r="O17" s="3">
         <v>19467</v>
       </c>
-      <c r="P17" s="28">
+      <c r="P17" s="19">
         <v>19483</v>
       </c>
       <c r="R17" s="3">
@@ -21534,7 +20973,7 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="3">
         <v>20169</v>
       </c>
@@ -21568,7 +21007,7 @@
       <c r="O18" s="3">
         <v>19479</v>
       </c>
-      <c r="P18" s="28">
+      <c r="P18" s="19">
         <v>19489</v>
       </c>
       <c r="R18" s="3">
@@ -21585,7 +21024,7 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="3">
         <v>20101</v>
       </c>
@@ -21619,7 +21058,7 @@
       <c r="O19" s="3">
         <v>19494</v>
       </c>
-      <c r="P19" s="28">
+      <c r="P19" s="19">
         <v>19457</v>
       </c>
       <c r="R19" s="3">
@@ -21636,7 +21075,7 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="3">
         <v>20133</v>
       </c>
@@ -21670,7 +21109,7 @@
       <c r="O20" s="3">
         <v>19472</v>
       </c>
-      <c r="P20" s="28">
+      <c r="P20" s="19">
         <v>19482</v>
       </c>
       <c r="R20" s="3">
@@ -21687,7 +21126,7 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="38"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="3">
         <v>20144</v>
       </c>
@@ -21721,7 +21160,7 @@
       <c r="O21" s="3">
         <v>19501</v>
       </c>
-      <c r="P21" s="28">
+      <c r="P21" s="19">
         <v>19469</v>
       </c>
       <c r="R21" s="3">
@@ -21738,7 +21177,7 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="38"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="3">
         <v>20103</v>
       </c>
@@ -21772,7 +21211,7 @@
       <c r="O22" s="3">
         <v>19501</v>
       </c>
-      <c r="P22" s="28">
+      <c r="P22" s="19">
         <v>19477</v>
       </c>
       <c r="R22" s="3">
@@ -21789,7 +21228,7 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="38"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="3">
         <v>20169</v>
       </c>
@@ -21823,7 +21262,7 @@
       <c r="O23" s="3">
         <v>19490</v>
       </c>
-      <c r="P23" s="28">
+      <c r="P23" s="19">
         <v>19463</v>
       </c>
       <c r="R23" s="3">
@@ -21840,7 +21279,7 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="3">
         <v>20100</v>
       </c>
@@ -21874,7 +21313,7 @@
       <c r="O24" s="3">
         <v>19482</v>
       </c>
-      <c r="P24" s="28">
+      <c r="P24" s="19">
         <v>19465</v>
       </c>
       <c r="R24" s="3">
@@ -21891,7 +21330,7 @@
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="3">
         <v>20115</v>
       </c>
@@ -21925,7 +21364,7 @@
       <c r="O25" s="3">
         <v>19498</v>
       </c>
-      <c r="P25" s="28">
+      <c r="P25" s="19">
         <v>19489</v>
       </c>
       <c r="R25" s="3">
@@ -21942,7 +21381,7 @@
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="3">
@@ -22011,7 +21450,7 @@
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="41" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="3">
@@ -22023,7 +21462,7 @@
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="40"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="3">
         <f>(D6+D7+D8+D9+D10+D11+D12+D13+D14+D15+D16+D17+D18+D19+D20+D21+D22+D23+D24+D25)/20</f>
         <v>20120.8</v>
@@ -22033,7 +21472,7 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="3">
         <f>(E6+E7+E8+E9+E10+E11+E12+E13+E14+E15+E16+E17+E18+E19+E20+E21+E22+E23+E24+E25)/20</f>
         <v>20107.45</v>
@@ -22043,7 +21482,7 @@
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B32" s="41"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="3">
         <f>(F6+F7+F8+F9+F10+F11+F12+F13+F14+F15+F16+F17+F18+F19+F20+F21+F22+F23+F24+F25)/20</f>
         <v>20084.599999999999</v>
@@ -22053,36 +21492,36 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="29"/>
+      <c r="B33" s="20"/>
       <c r="D33" s="7"/>
       <c r="E33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="29"/>
+      <c r="B34" s="20"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
+      <c r="B35" s="20"/>
       <c r="D35" s="7"/>
       <c r="E35">
         <v>299</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="29"/>
+      <c r="B36" s="20"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="29"/>
+      <c r="B37" s="20"/>
       <c r="D37" s="7"/>
       <c r="E37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="3">
@@ -22094,7 +21533,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="40"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="3">
         <f>(I6+I7+I8+I9+I10+I11+I12+I13+I14+I15+I16+I17+I18+I19+I20+I21+I22+I23+I24+I25)/20</f>
         <v>20011.400000000001</v>
@@ -22104,7 +21543,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="40"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="3">
         <f>(J6+J7+J8+J9+J10+J11+J12+J13+J14+J15+J16+J17+J18+J19+J20+J21+J22+J23+J24+J25)/20</f>
         <v>19950.599999999999</v>
@@ -22114,7 +21553,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="41"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="3">
         <f>(K6+K7+K8+K9+K10+K11+K12+K13+K14+K15+K16+K17+K18+K19+K20+K21+K22+K23+K24+K25)/20</f>
         <v>19838.099999999999</v>
@@ -22124,7 +21563,7 @@
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="29"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" t="s">
@@ -22132,7 +21571,7 @@
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="29"/>
+      <c r="B43" s="20"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43">
@@ -22140,12 +21579,12 @@
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
+      <c r="B44" s="21"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" t="s">
@@ -22153,7 +21592,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="41" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="3">
@@ -22165,7 +21604,7 @@
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="40"/>
+      <c r="B47" s="42"/>
       <c r="C47" s="3">
         <f>(N6+N7+N8+N9+N10+N11+N12+N13+N14+N15+N16+N17+N18+N19+N20+N21+N22+N23+N24+N25)/20</f>
         <v>19663.849999999999</v>
@@ -22175,7 +21614,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="40"/>
+      <c r="B48" s="42"/>
       <c r="C48" s="3">
         <f>(O6+O7+O8+O9+O10+O11+O12+O13+O14+O15+O16+O17+O18+O19+O20+O21+O22+O23+O24+O25)/20</f>
         <v>19486.5</v>
@@ -22185,7 +21624,7 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="41"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="3">
         <f>(P6+P7+P8+P9+P10+P11+P12+P13+P14+P15+P16+P17+P18+P19+P20+P21+P22+P23+P24+P25)/20</f>
         <v>19472.099999999999</v>
@@ -22195,32 +21634,32 @@
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="30"/>
+      <c r="B50" s="21"/>
       <c r="D50" s="7"/>
       <c r="E50" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="30"/>
+      <c r="B51" s="21"/>
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="30"/>
+      <c r="B52" s="21"/>
       <c r="D52" s="7"/>
       <c r="E52">
         <v>799</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="30"/>
+      <c r="B53" s="21"/>
       <c r="D53" s="7"/>
       <c r="E53">
         <v>19521</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="41" t="s">
         <v>32</v>
       </c>
       <c r="C54" s="2">
@@ -22232,7 +21671,7 @@
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="40"/>
+      <c r="B55" s="42"/>
       <c r="C55" s="2">
         <f>(S6+S7+S8+S9+S10+S11+S12+S13+S14+S15+S16+S17+S18+S19+S20+S21+S22+S23+S24+S25)/20</f>
         <v>18965.849999999999</v>
@@ -22242,7 +21681,7 @@
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="40"/>
+      <c r="B56" s="42"/>
       <c r="C56" s="2">
         <f>(T6+T7+T8+T9+T10+T11+T12+T13+T14+T15+T16+T17+T18+T19+T20+T21+T22+T23+T24+T25)/20</f>
         <v>18418.45</v>
@@ -22252,7 +21691,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="41"/>
+      <c r="B57" s="43"/>
       <c r="C57" s="2">
         <f>(U6+U7+U8+U9+U10+U11+U12+U13+U14+U15+U16+U17+U18+U19+U20+U21+U22+U23+U24+U25)/20</f>
         <v>17900.349999999999</v>

</xml_diff>